<commit_message>
added deliverables and syllabus
</commit_message>
<xml_diff>
--- a/data/AD698-Schedule.xlsx
+++ b/data/AD698-Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\AD698-generative-ai-for-BA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C655CE-4D39-4388-8296-7BA331DFED7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77576649-D1B6-4D1E-A580-98671C176B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{289CF049-F2D7-49EE-A36E-C623D66A4696}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="225">
   <si>
     <t>Assignment</t>
   </si>
@@ -275,54 +275,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Overview of course objectives and use of GenAI in business contexts.</t>
-  </si>
-  <si>
-    <t>Setup instructions for local development using GitHub, Jupyter, and APIs.</t>
-  </si>
-  <si>
-    <t>Core prompting strategies including few-shot, CoT, and ReAct.</t>
-  </si>
-  <si>
-    <t>Applying prompt templates to generate emails, reports, SQL, and summaries.</t>
-  </si>
-  <si>
-    <t>Understanding vector databases and embedding models for RAG.</t>
-  </si>
-  <si>
-    <t>Implementing retrieval-based Q&amp;A systems using LangChain and LlamaIndex.</t>
-  </si>
-  <si>
-    <t>Introduction to AI agents and tool-use chains with LangChain.</t>
-  </si>
-  <si>
-    <t>Designing multi-agent systems for business process automation.</t>
-  </si>
-  <si>
-    <t>Overview of parameter-efficient tuning strategies for LLMs.</t>
-  </si>
-  <si>
-    <t>Running LoRA/QLoRA fine-tunes and comparing to base models.</t>
-  </si>
-  <si>
-    <t>Using embedding models for semantic similarity and clustering.</t>
-  </si>
-  <si>
-    <t>Building memory modules to preserve context in long tasks.</t>
-  </si>
-  <si>
-    <t>Evaluation methods for LLMs including hallucination and output quality.</t>
-  </si>
-  <si>
-    <t>Auditing AI outputs for bias, fairness, and responsible use.</t>
-  </si>
-  <si>
-    <t>Techniques for reducing model size and optimizing inference speed.</t>
-  </si>
-  <si>
-    <t>Deploying GenAI applications using GitHub Actions and Streamlit.</t>
-  </si>
-  <si>
     <t>Section</t>
   </si>
   <si>
@@ -633,6 +585,138 @@
   </si>
   <si>
     <t>Weekly Labs8</t>
+  </si>
+  <si>
+    <t>Dev Setup: GitHub, Jupyter, VS Code, Colab</t>
+  </si>
+  <si>
+    <t>Introduction to Neural Networks</t>
+  </si>
+  <si>
+    <t>Introduction to Natural Language Processing</t>
+  </si>
+  <si>
+    <t>Introduction to Course, Natural Language, and Generative AI Landscape</t>
+  </si>
+  <si>
+    <t>Course tools setup and basic version control with GitHub, notebooks, and IDEs.</t>
+  </si>
+  <si>
+    <t>Understanding the basics of neural networks as a foundation for generative models.</t>
+  </si>
+  <si>
+    <t>Overview of generative AI, its business relevance, and natural language as a data type.</t>
+  </si>
+  <si>
+    <t>Core NLP concepts: tokenization, POS tagging, parsing, and text pre-processing.</t>
+  </si>
+  <si>
+    <t>Learn prompt design, zero-/few-shot techniques, and ICL with business use cases.</t>
+  </si>
+  <si>
+    <t>Tokenization, Embeddings, and Vector Semantics</t>
+  </si>
+  <si>
+    <t>Deep dive into tokenization methods, word embeddings, and semantic search foundations.</t>
+  </si>
+  <si>
+    <t>LLM Internals: Attention, Transformers, and Positional Encoding</t>
+  </si>
+  <si>
+    <t>Explore transformer architecture, attention mechanisms, and context windows.</t>
+  </si>
+  <si>
+    <t>Understanding retrieval-augmented generation concepts and corpus preparation.</t>
+  </si>
+  <si>
+    <t>Build Q&amp;A systems using vector DBs, LangChain chains, and document loaders.</t>
+  </si>
+  <si>
+    <t>Overview of agent-based systems and tool-augmented LLM workflows.</t>
+  </si>
+  <si>
+    <t>Design and orchestrate multi-agent collaborative systems for enterprise tasks.</t>
+  </si>
+  <si>
+    <t>Learn parameter-efficient fine-tuning methods to adapt base models.</t>
+  </si>
+  <si>
+    <t>Set up custom model pipelines and format datasets for supervised fine-tuning.</t>
+  </si>
+  <si>
+    <t>Work with sentence embeddings for document clustering, search, and relevance.</t>
+  </si>
+  <si>
+    <t>Strategies for working with limited context: caching, summaries, and memory buffers.</t>
+  </si>
+  <si>
+    <t>Evaluate generated outputs using automated tools, manual rubrics, and hallucination detection.</t>
+  </si>
+  <si>
+    <t>Assess bias, fairness, and ethics in generated outputs using toolkits and guidelines.</t>
+  </si>
+  <si>
+    <t>Multimodal Models and Use Cases</t>
+  </si>
+  <si>
+    <t>Explore vision-language models and multimodal business applications.</t>
+  </si>
+  <si>
+    <t>On-Campus</t>
+  </si>
+  <si>
+    <t>L0.1</t>
+  </si>
+  <si>
+    <t>L0.2</t>
+  </si>
+  <si>
+    <t>L1.1</t>
+  </si>
+  <si>
+    <t>L1.2</t>
+  </si>
+  <si>
+    <t>L2.1</t>
+  </si>
+  <si>
+    <t>L2.2</t>
+  </si>
+  <si>
+    <t>L3.1</t>
+  </si>
+  <si>
+    <t>L3.2</t>
+  </si>
+  <si>
+    <t>L4.1</t>
+  </si>
+  <si>
+    <t>L4.2</t>
+  </si>
+  <si>
+    <t>L5.1</t>
+  </si>
+  <si>
+    <t>L5.2</t>
+  </si>
+  <si>
+    <t>L6.1</t>
+  </si>
+  <si>
+    <t>L6.2</t>
+  </si>
+  <si>
+    <t>L7.1</t>
+  </si>
+  <si>
+    <t>L7.2</t>
+  </si>
+  <si>
+    <t>L8.1</t>
+  </si>
+  <si>
+    <t>L8.2</t>
   </si>
 </sst>
 </file>
@@ -877,22 +961,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1055,6 +1127,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1394,368 +1472,337 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B2A5D89-D79C-44C1-8747-841FF0601386}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9" style="58" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="58" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46" style="58" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.85546875" style="59" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="58" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="58" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="58"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="56" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D7" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="60" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="61" t="s">
-        <v>94</v>
-      </c>
-      <c r="D1" s="61" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="7" t="s">
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C8" t="s">
         <v>192</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="D8" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" s="62">
-        <v>45902</v>
-      </c>
-      <c r="F4" s="62">
-        <v>45908</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" s="62">
-        <v>45902</v>
-      </c>
-      <c r="F5" s="62">
-        <v>45915</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>199</v>
+      </c>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>215</v>
+      </c>
+      <c r="C10" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" s="62">
-        <v>45909</v>
-      </c>
-      <c r="F6" s="62">
-        <v>45922</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="D10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>216</v>
+      </c>
+      <c r="C11" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" s="62">
-        <v>45909</v>
-      </c>
-      <c r="F7" s="62">
-        <v>45929</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="D11" t="s">
+        <v>195</v>
+      </c>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>217</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>198</v>
+      </c>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
+        <v>218</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
+        <v>219</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>201</v>
+      </c>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
+        <v>220</v>
+      </c>
+      <c r="C15" t="s">
+        <v>204</v>
+      </c>
+      <c r="D15" t="s">
+        <v>205</v>
+      </c>
+      <c r="E15" s="60"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
+        <v>221</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
+        <v>202</v>
+      </c>
+      <c r="E16" s="60"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
+        <v>222</v>
+      </c>
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" t="s">
+        <v>203</v>
+      </c>
+      <c r="E17" s="60"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
+        <v>223</v>
+      </c>
+      <c r="C18" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E8" s="62">
-        <v>45916</v>
-      </c>
-      <c r="F8" s="62">
-        <v>45936</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="D18" t="s">
+        <v>196</v>
+      </c>
+      <c r="E18" s="60"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" t="s">
+        <v>224</v>
+      </c>
+      <c r="C19" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" s="62">
-        <v>45916</v>
-      </c>
-      <c r="F9" s="62">
-        <v>45950</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E10" s="62">
-        <v>45923</v>
-      </c>
-      <c r="F10" s="62">
-        <v>45957</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E11" s="62">
-        <v>45923</v>
-      </c>
-      <c r="F11" s="62">
-        <v>45964</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E12" s="62">
-        <v>45930</v>
-      </c>
-      <c r="F12" s="62">
-        <v>45971</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E13" s="62">
-        <v>45930</v>
-      </c>
-      <c r="F13" s="62">
-        <v>45978</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="E14" s="62">
-        <v>45937</v>
-      </c>
-      <c r="F14" s="62">
-        <v>45985</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E15" s="62">
-        <v>45937</v>
-      </c>
-      <c r="F15" s="62">
-        <v>45992</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="62">
-        <v>45999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>74</v>
-      </c>
+      <c r="D19" t="s">
+        <v>197</v>
+      </c>
+      <c r="E19" s="60"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="60"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="60"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="60"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="60"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1772,63 +1819,63 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="8" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>97</v>
+      <c r="A1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E2" s="59">
+      <c r="A2" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="55">
         <v>0.60416666666666663</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>103</v>
+      <c r="A3" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1848,241 +1895,241 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="7" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1"/>
-    <col min="5" max="5" width="46.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="16"/>
+    <col min="5" max="5" width="46.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>110</v>
+        <v>88</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="13">
+        <v>95</v>
+      </c>
+      <c r="B2" s="9">
         <f>F2+F3</f>
         <v>2</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="9">
         <f>H2+H3</f>
         <v>140</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="F2" s="13">
+      <c r="E2" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="F2" s="9">
         <v>1</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="9">
         <v>100</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="10">
         <f>F2*G2</f>
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>196</v>
-      </c>
-      <c r="B3" s="13">
+        <v>180</v>
+      </c>
+      <c r="B3" s="9">
         <f>F4</f>
         <v>10</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="9">
         <f>H4</f>
         <v>200</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="F3" s="13">
+      <c r="E3" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="9">
         <v>1</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="9">
         <v>40</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="10">
         <f>F3*G3</f>
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B4" s="13">
+        <v>97</v>
+      </c>
+      <c r="B4" s="9">
         <f>F5</f>
         <v>5</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="9">
         <f>H5</f>
         <v>250</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="F4" s="13">
+      <c r="E4" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="F4" s="9">
         <v>10</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="9">
         <v>20</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="10">
         <f>F4*G4</f>
         <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" s="13">
+        <v>99</v>
+      </c>
+      <c r="B5" s="9">
         <f>SUM(F7:F10)</f>
         <v>4</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="9">
         <f>H6+H11+H12</f>
         <v>160</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="9">
         <v>5</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="9">
         <v>50</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="10">
         <f>F5*G5</f>
         <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C6" s="13">
+        <v>106</v>
+      </c>
+      <c r="C6" s="9">
         <f>SUM(C2:C5)</f>
         <v>750</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="F6" s="13">
+      <c r="E6" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="F6" s="9">
         <v>1</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="9">
         <v>80</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="10">
         <f>F6*G6</f>
         <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E7" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="F7" s="13">
+      <c r="E7" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" s="9">
         <v>1</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="14"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E8" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="F8" s="13">
+      <c r="E8" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="9">
         <v>1</v>
       </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="14"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E9" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F9" s="13">
+      <c r="E9" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="9">
         <v>1</v>
       </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="14"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E10" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="F10" s="13">
+      <c r="E10" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F10" s="9">
         <v>1</v>
       </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="14"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>120</v>
-      </c>
-      <c r="F11" s="13">
+        <v>104</v>
+      </c>
+      <c r="F11" s="9">
         <v>1</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="9">
         <v>40</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="10">
         <f>F11*G11</f>
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>121</v>
-      </c>
-      <c r="F12" s="13">
+        <v>105</v>
+      </c>
+      <c r="F12" s="9">
         <v>1</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="9">
         <v>40</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="10">
         <f>F12*G12</f>
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E13" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13">
+      <c r="E13" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9">
         <f>SUM(H2:H12)</f>
         <v>750</v>
       </c>
@@ -2103,112 +2150,112 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>124</v>
+      <c r="A1" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="18">
+      <c r="A2" s="14">
         <v>45678</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="14">
         <v>45680</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="14">
         <v>45679</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="18">
+      <c r="A3" s="14">
         <f>A2+1</f>
         <v>45679</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="14">
         <f t="shared" ref="B3:C8" si="0">B2+1</f>
         <v>45681</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="14">
         <f t="shared" si="0"/>
         <v>45680</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="18">
+      <c r="A4" s="14">
         <f t="shared" ref="A4:A8" si="1">A3+1</f>
         <v>45680</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="14">
         <f t="shared" si="0"/>
         <v>45682</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="14">
         <f t="shared" si="0"/>
         <v>45681</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="18">
+      <c r="A5" s="14">
         <f t="shared" si="1"/>
         <v>45681</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="14">
         <f t="shared" si="0"/>
         <v>45683</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="14">
         <f t="shared" si="0"/>
         <v>45682</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="18">
+      <c r="A6" s="14">
         <f t="shared" si="1"/>
         <v>45682</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="14">
         <f t="shared" si="0"/>
         <v>45684</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="14">
         <f t="shared" si="0"/>
         <v>45683</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
+      <c r="A7" s="14">
         <f t="shared" si="1"/>
         <v>45683</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="14">
         <f t="shared" si="0"/>
         <v>45685</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="14">
         <f t="shared" si="0"/>
         <v>45684</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="18">
+      <c r="A8" s="14">
         <f t="shared" si="1"/>
         <v>45684</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="14">
         <f t="shared" si="0"/>
         <v>45686</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="14">
         <f t="shared" si="0"/>
         <v>45685</v>
       </c>
@@ -2229,217 +2276,217 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="11.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="11.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="10.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="24"/>
+    <col min="1" max="1" width="11.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="11.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="11.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="10.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="P1" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q1" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="R1" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="S1" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="T1" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="19" t="s">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="B2" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="F1" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="G1" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="E2" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="J1" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="K1" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="L1" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="M1" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="N1" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="O1" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="P1" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q1" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="R1" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="S1" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="T1" s="23" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="F2" s="27">
+      <c r="F2" s="23">
         <v>0.60416666666666663</v>
       </c>
-      <c r="G2" s="28">
+      <c r="G2" s="24">
         <v>45908</v>
       </c>
-      <c r="H2" s="28">
+      <c r="H2" s="24">
         <f>G2+7</f>
         <v>45915</v>
       </c>
-      <c r="I2" s="28">
+      <c r="I2" s="24">
         <f t="shared" ref="I2:J3" si="0">H2+7</f>
         <v>45922</v>
       </c>
-      <c r="J2" s="28">
+      <c r="J2" s="24">
         <f t="shared" si="0"/>
         <v>45929</v>
       </c>
-      <c r="K2" s="28">
+      <c r="K2" s="24">
         <f>J2+14</f>
         <v>45943</v>
       </c>
-      <c r="L2" s="28">
+      <c r="L2" s="24">
         <f>K2+7</f>
         <v>45950</v>
       </c>
-      <c r="M2" s="28">
+      <c r="M2" s="24">
         <f>L2+14</f>
         <v>45964</v>
       </c>
-      <c r="N2" s="28">
+      <c r="N2" s="24">
         <f t="shared" ref="N2:S2" si="1">M2+7</f>
         <v>45971</v>
       </c>
-      <c r="O2" s="28">
+      <c r="O2" s="24">
         <f t="shared" si="1"/>
         <v>45978</v>
       </c>
-      <c r="P2" s="28">
+      <c r="P2" s="24">
         <f t="shared" si="1"/>
         <v>45985</v>
       </c>
-      <c r="Q2" s="28">
+      <c r="Q2" s="24">
         <f t="shared" si="1"/>
         <v>45992</v>
       </c>
-      <c r="R2" s="28">
+      <c r="R2" s="24">
         <f t="shared" si="1"/>
         <v>45999</v>
       </c>
-      <c r="S2" s="28">
+      <c r="S2" s="24">
         <f t="shared" si="1"/>
         <v>46006</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="F3" s="29">
+      <c r="A3" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="F3" s="25">
         <v>0.79166666666666663</v>
       </c>
-      <c r="G3" s="28">
+      <c r="G3" s="24">
         <v>45902</v>
       </c>
-      <c r="H3" s="28">
+      <c r="H3" s="24">
         <f>G3+7</f>
         <v>45909</v>
       </c>
-      <c r="I3" s="28">
+      <c r="I3" s="24">
         <f t="shared" si="0"/>
         <v>45916</v>
       </c>
-      <c r="J3" s="28">
+      <c r="J3" s="24">
         <f t="shared" si="0"/>
         <v>45923</v>
       </c>
-      <c r="K3" s="28">
+      <c r="K3" s="24">
         <f>J3+14</f>
         <v>45937</v>
       </c>
-      <c r="L3" s="28">
+      <c r="L3" s="24">
         <f>K3+7</f>
         <v>45944</v>
       </c>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="24"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="22"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="26"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2461,669 +2508,669 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" style="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" style="49" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" style="49" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" style="49" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" style="49" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.28515625" style="49" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" style="49" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="49" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.28515625" style="49" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="49" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" style="49" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.5703125" style="49" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.28515625" style="49" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="35"/>
+    <col min="1" max="1" width="9.5703125" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" style="45" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" style="45" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="45" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" style="45" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="45" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" style="45" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" style="45" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="45" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.28515625" style="45" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="45" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" style="45" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.5703125" style="45" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.28515625" style="45" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="P1" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q1" s="19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="E2" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="C1" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="D1" s="22" t="s">
+      <c r="F2" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="G2" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="H2" s="33"/>
+      <c r="I2" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="J2" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="K2" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="L2" s="33"/>
+      <c r="M2" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="34"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="D3" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="J3" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="K3" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="36"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="D4" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="J4" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="K4" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="36"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="B5" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="39"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="41"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="C6" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="G6" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="O1" s="22" t="s">
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="K6" s="33" t="s">
         <v>164</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="L6" s="46"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33" t="s">
         <v>165</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="P6" s="47"/>
+      <c r="Q6" s="48"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="G7" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="K7" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="50"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="G8" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="K8" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="50"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
+        <v>161</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="C9" s="39"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="52"/>
+      <c r="P9" s="52"/>
+      <c r="Q9" s="53"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>150</v>
-      </c>
-      <c r="D2" s="37" t="s">
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33" t="s">
         <v>168</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="O10" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37" t="s">
+      <c r="P10" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q10" s="34"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="O11" s="35" t="s">
+        <v>170</v>
+      </c>
+      <c r="P11" s="35" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q11" s="36"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="L12" s="35"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="O12" s="35" t="s">
+        <v>170</v>
+      </c>
+      <c r="P12" s="35" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q12" s="36"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="37" t="s">
+        <v>161</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="39"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="41"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="43" t="s">
         <v>171</v>
       </c>
-      <c r="J2" s="37" t="s">
+      <c r="C14" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="N14" s="33"/>
+      <c r="O14" s="33"/>
+      <c r="P14" s="33"/>
+      <c r="Q14" s="34"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="N15" s="35"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="36"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="N16" s="35"/>
+      <c r="O16" s="35"/>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="36"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="37" t="s">
+        <v>161</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="C17" s="39"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="N17" s="40"/>
+      <c r="O17" s="40"/>
+      <c r="P17" s="40"/>
+      <c r="Q17" s="41"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="K2" s="37" t="s">
-        <v>173</v>
-      </c>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37" t="s">
-        <v>174</v>
-      </c>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="38"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>175</v>
-      </c>
-      <c r="D3" s="39" t="s">
-        <v>167</v>
-      </c>
-      <c r="E3" s="39" t="s">
-        <v>168</v>
-      </c>
-      <c r="F3" s="39" t="s">
-        <v>169</v>
-      </c>
-      <c r="G3" s="39" t="s">
-        <v>170</v>
-      </c>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39" t="s">
-        <v>171</v>
-      </c>
-      <c r="J3" s="39" t="s">
+      <c r="C18" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="N18" s="35"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="36"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="K3" s="39" t="s">
-        <v>173</v>
-      </c>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39" t="s">
-        <v>174</v>
-      </c>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="40"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="B4" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>176</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>167</v>
-      </c>
-      <c r="E4" s="39" t="s">
-        <v>168</v>
-      </c>
-      <c r="F4" s="39" t="s">
-        <v>169</v>
-      </c>
-      <c r="G4" s="39" t="s">
-        <v>170</v>
-      </c>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39" t="s">
-        <v>171</v>
-      </c>
-      <c r="J4" s="39" t="s">
+      <c r="C19" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="D19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="N19" s="35"/>
+      <c r="O19" s="35"/>
+      <c r="P19" s="35"/>
+      <c r="Q19" s="36"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="K4" s="39" t="s">
-        <v>173</v>
-      </c>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39" t="s">
-        <v>174</v>
-      </c>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="40"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
-        <v>177</v>
-      </c>
-      <c r="B5" s="42" t="s">
-        <v>114</v>
-      </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
-      <c r="N5" s="44"/>
-      <c r="O5" s="44"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="45"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6" s="47" t="s">
-        <v>178</v>
-      </c>
-      <c r="C6" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="G6" s="37" t="s">
-        <v>179</v>
-      </c>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="K6" s="37" t="s">
-        <v>180</v>
-      </c>
-      <c r="L6" s="50"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37" t="s">
-        <v>181</v>
-      </c>
-      <c r="P6" s="51"/>
-      <c r="Q6" s="52"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="B7" s="35" t="s">
-        <v>178</v>
-      </c>
-      <c r="C7" s="36" t="s">
-        <v>175</v>
-      </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="G7" s="39" t="s">
-        <v>179</v>
-      </c>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="K7" s="39" t="s">
-        <v>180</v>
-      </c>
-      <c r="M7" s="39"/>
-      <c r="N7" s="39" t="s">
-        <v>181</v>
-      </c>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="54"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="B8" s="35" t="s">
-        <v>178</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>176</v>
-      </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="G8" s="39" t="s">
-        <v>179</v>
-      </c>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="K8" s="39" t="s">
-        <v>180</v>
-      </c>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39" t="s">
-        <v>181</v>
-      </c>
-      <c r="P8" s="53"/>
-      <c r="Q8" s="54"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
-        <v>177</v>
-      </c>
-      <c r="B9" s="42" t="s">
-        <v>178</v>
-      </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="44"/>
-      <c r="O9" s="56"/>
-      <c r="P9" s="56"/>
-      <c r="Q9" s="57"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="B10" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37" t="s">
-        <v>182</v>
-      </c>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37" t="s">
-        <v>183</v>
-      </c>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="L10" s="37"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="37" t="s">
-        <v>185</v>
-      </c>
-      <c r="O10" s="37" t="s">
-        <v>186</v>
-      </c>
-      <c r="P10" s="37" t="s">
-        <v>186</v>
-      </c>
-      <c r="Q10" s="38"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="B11" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>175</v>
-      </c>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39" t="s">
-        <v>182</v>
-      </c>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39" t="s">
-        <v>183</v>
-      </c>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39" t="s">
-        <v>184</v>
-      </c>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39" t="s">
-        <v>185</v>
-      </c>
-      <c r="O11" s="39" t="s">
-        <v>186</v>
-      </c>
-      <c r="P11" s="39" t="s">
-        <v>186</v>
-      </c>
-      <c r="Q11" s="40"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="B12" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>176</v>
-      </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39" t="s">
-        <v>182</v>
-      </c>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39" t="s">
-        <v>183</v>
-      </c>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39" t="s">
-        <v>184</v>
-      </c>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39" t="s">
-        <v>185</v>
-      </c>
-      <c r="O12" s="39" t="s">
-        <v>186</v>
-      </c>
-      <c r="P12" s="39" t="s">
-        <v>186</v>
-      </c>
-      <c r="Q12" s="40"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="41" t="s">
-        <v>177</v>
-      </c>
-      <c r="B13" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="44"/>
-      <c r="O13" s="44"/>
-      <c r="P13" s="44"/>
-      <c r="Q13" s="45"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="B14" s="47" t="s">
-        <v>187</v>
-      </c>
-      <c r="C14" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37" t="s">
-        <v>162</v>
-      </c>
-      <c r="N14" s="37"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="38"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="B15" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="C15" s="36" t="s">
-        <v>175</v>
-      </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="39" t="s">
-        <v>162</v>
-      </c>
-      <c r="N15" s="39"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="40"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="B16" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="C16" s="36" t="s">
-        <v>176</v>
-      </c>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39" t="s">
-        <v>162</v>
-      </c>
-      <c r="N16" s="39"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="40"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="41" t="s">
-        <v>177</v>
-      </c>
-      <c r="B17" s="42" t="s">
-        <v>187</v>
-      </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="44"/>
-      <c r="K17" s="44"/>
-      <c r="L17" s="44"/>
-      <c r="M17" s="44" t="s">
-        <v>162</v>
-      </c>
-      <c r="N17" s="44"/>
-      <c r="O17" s="44"/>
-      <c r="P17" s="44"/>
-      <c r="Q17" s="45"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="B18" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="C18" s="36" t="s">
-        <v>150</v>
-      </c>
-      <c r="D18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="39" t="s">
-        <v>162</v>
-      </c>
-      <c r="N18" s="39"/>
-      <c r="O18" s="39"/>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="40"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="B19" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="C19" s="36" t="s">
-        <v>175</v>
-      </c>
-      <c r="D19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="39" t="s">
-        <v>162</v>
-      </c>
-      <c r="N19" s="39"/>
-      <c r="O19" s="39"/>
-      <c r="P19" s="39"/>
-      <c r="Q19" s="40"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="B20" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="C20" s="36" t="s">
-        <v>176</v>
-      </c>
-      <c r="D20" s="39"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39" t="s">
-        <v>162</v>
-      </c>
-      <c r="N20" s="39"/>
-      <c r="O20" s="39"/>
-      <c r="P20" s="39"/>
-      <c r="Q20" s="40"/>
+      <c r="C20" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="D20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="N20" s="35"/>
+      <c r="O20" s="35"/>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="36"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="41" t="s">
-        <v>177</v>
-      </c>
-      <c r="B21" s="42" t="s">
-        <v>188</v>
-      </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="44" t="s">
-        <v>162</v>
-      </c>
-      <c r="N21" s="44"/>
-      <c r="O21" s="44"/>
-      <c r="P21" s="44"/>
-      <c r="Q21" s="45"/>
+      <c r="A21" s="37" t="s">
+        <v>161</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3150,42 +3197,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
-        <v>191</v>
-      </c>
-      <c r="B1" s="60" t="s">
+      <c r="A1" s="56" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="61" t="s">
-        <v>94</v>
-      </c>
-      <c r="D1" s="61" t="s">
+      <c r="C1" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>193</v>
+      <c r="E1" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -3439,20 +3486,20 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2" t="s">
+      <c r="D19" s="1"/>
+      <c r="E19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added course structure to excel
</commit_message>
<xml_diff>
--- a/data/AD698-Schedule.xlsx
+++ b/data/AD698-Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\AD698-generative-ai-for-BA\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npadalka\Documents\Repositories\AD698-generative-ai-for-BA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77576649-D1B6-4D1E-A580-98671C176B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CB9708-DF79-429C-A3F0-7990A0884EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{289CF049-F2D7-49EE-A36E-C623D66A4696}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" activeTab="2" xr2:uid="{289CF049-F2D7-49EE-A36E-C623D66A4696}"/>
   </bookViews>
   <sheets>
     <sheet name="Course Details" sheetId="2" r:id="rId1"/>
@@ -584,9 +584,6 @@
     <t>Labs*</t>
   </si>
   <si>
-    <t>Weekly Labs8</t>
-  </si>
-  <si>
     <t>Dev Setup: GitHub, Jupyter, VS Code, Colab</t>
   </si>
   <si>
@@ -717,6 +714,9 @@
   </si>
   <si>
     <t>L8.2</t>
+  </si>
+  <si>
+    <t>Weekly Labs*</t>
   </si>
 </sst>
 </file>
@@ -1474,22 +1474,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B2A5D89-D79C-44C1-8747-841FF0601386}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9" style="58" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="58" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" style="58" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" style="58" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.85546875" style="59" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="58" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="58"/>
+    <col min="4" max="4" width="52.81640625" style="59" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" style="58" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7265625" style="58" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="56" t="s">
         <v>175</v>
       </c>
@@ -1506,302 +1506,302 @@
         <v>176</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E2" s="60"/>
       <c r="F2" s="60"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E3" s="60"/>
       <c r="F3" s="60"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E6" s="60"/>
       <c r="F6" s="60"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D7" t="s">
         <v>190</v>
-      </c>
-      <c r="D7" t="s">
-        <v>191</v>
       </c>
       <c r="E7" s="60"/>
       <c r="F7" s="60"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C8" t="s">
+        <v>191</v>
+      </c>
+      <c r="D8" t="s">
         <v>192</v>
-      </c>
-      <c r="D8" t="s">
-        <v>193</v>
       </c>
       <c r="E8" s="60"/>
       <c r="F8" s="60"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C9" t="s">
         <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E9" s="60"/>
       <c r="F9" s="60"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E10" s="60"/>
       <c r="F10" s="60"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C11" t="s">
         <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E11" s="60"/>
       <c r="F11" s="60"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C12" t="s">
         <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E12" s="60"/>
       <c r="F12" s="60"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C13" t="s">
         <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E13" s="60"/>
       <c r="F13" s="60"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C14" t="s">
         <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E14" s="60"/>
       <c r="F14" s="60"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C15" t="s">
+        <v>203</v>
+      </c>
+      <c r="D15" t="s">
         <v>204</v>
       </c>
-      <c r="D15" t="s">
-        <v>205</v>
-      </c>
       <c r="E15" s="60"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C16" t="s">
         <v>55</v>
       </c>
       <c r="D16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E16" s="60"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C17" t="s">
         <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E17" s="60"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C18" t="s">
         <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E18" s="60"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>69</v>
       </c>
       <c r="B19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C19" t="s">
         <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E19" s="60"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E20" s="60"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E21" s="60"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E22" s="60"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E23" s="60"/>
     </row>
   </sheetData>
@@ -1817,17 +1817,17 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="5"/>
+    <col min="2" max="2" width="27.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>77</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="54" t="s">
         <v>82</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>0.60416666666666663</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="54" t="s">
         <v>85</v>
       </c>
@@ -1888,23 +1888,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC9F4A2C-504E-4299-BCAC-273B4ED698AA}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1"/>
-    <col min="5" max="5" width="46.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="12"/>
+    <col min="1" max="1" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.26953125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="25.26953125" customWidth="1"/>
+    <col min="5" max="5" width="46.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.1796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.1796875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="9.1796875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>95</v>
       </c>
@@ -1953,9 +1953,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>224</v>
       </c>
       <c r="B3" s="9">
         <f>F4</f>
@@ -1979,7 +1979,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>97</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>106</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E7" s="11" t="s">
         <v>100</v>
       </c>
@@ -2063,7 +2063,7 @@
       <c r="G7" s="9"/>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E8" s="11" t="s">
         <v>101</v>
       </c>
@@ -2073,7 +2073,7 @@
       <c r="G8" s="9"/>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E9" s="11" t="s">
         <v>102</v>
       </c>
@@ -2083,7 +2083,7 @@
       <c r="G9" s="9"/>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E10" s="11" t="s">
         <v>103</v>
       </c>
@@ -2093,7 +2093,7 @@
       <c r="G10" s="9"/>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E11" t="s">
         <v>104</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E12" t="s">
         <v>105</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E13" s="8" t="s">
         <v>106</v>
       </c>
@@ -2148,13 +2148,13 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>82</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="14">
         <v>45678</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>45679</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="14">
         <f>A2+1</f>
         <v>45679</v>
@@ -2190,7 +2190,7 @@
         <v>45680</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="14">
         <f t="shared" ref="A4:A8" si="1">A3+1</f>
         <v>45680</v>
@@ -2204,7 +2204,7 @@
         <v>45681</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="14">
         <f t="shared" si="1"/>
         <v>45681</v>
@@ -2218,7 +2218,7 @@
         <v>45682</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="14">
         <f t="shared" si="1"/>
         <v>45682</v>
@@ -2232,7 +2232,7 @@
         <v>45683</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="14">
         <f t="shared" si="1"/>
         <v>45683</v>
@@ -2246,7 +2246,7 @@
         <v>45684</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="14">
         <f t="shared" si="1"/>
         <v>45684</v>
@@ -2271,28 +2271,28 @@
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="G3" sqref="G2:L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="11.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="11.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="10.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="20"/>
+    <col min="1" max="1" width="11.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="11.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="11.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="10.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.1796875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>109</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>128</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>46006</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>133</v>
       </c>
@@ -2476,13 +2476,13 @@
       <c r="S3" s="24"/>
       <c r="T3" s="24"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
       <c r="D4" s="21"/>
       <c r="E4" s="22"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B5" s="22"/>
       <c r="C5" s="22"/>
       <c r="D5" s="21"/>
@@ -2506,28 +2506,28 @@
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" style="45" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" style="45" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.54296875" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.26953125" style="45" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1796875" style="45" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="45" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" style="45" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" style="45" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.28515625" style="45" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.26953125" style="45" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1796875" style="45" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.26953125" style="45" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" style="45" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="45" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.28515625" style="45" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="45" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.1796875" style="45" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.26953125" style="45" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.453125" style="45" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10" style="45" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.5703125" style="45" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.28515625" style="45" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="31"/>
+    <col min="15" max="16" width="10.54296875" style="45" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.26953125" style="45" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.1796875" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>135</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="30" t="s">
         <v>82</v>
       </c>
@@ -2621,7 +2621,7 @@
       <c r="P2" s="33"/>
       <c r="Q2" s="34"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="30" t="s">
         <v>107</v>
       </c>
@@ -2662,7 +2662,7 @@
       <c r="P3" s="35"/>
       <c r="Q3" s="36"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="30" t="s">
         <v>108</v>
       </c>
@@ -2703,7 +2703,7 @@
       <c r="P4" s="35"/>
       <c r="Q4" s="36"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="37" t="s">
         <v>161</v>
       </c>
@@ -2726,7 +2726,7 @@
       <c r="P5" s="40"/>
       <c r="Q5" s="41"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="42" t="s">
         <v>82</v>
       </c>
@@ -2754,7 +2754,7 @@
       <c r="P6" s="47"/>
       <c r="Q6" s="48"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="30" t="s">
         <v>107</v>
       </c>
@@ -2781,7 +2781,7 @@
       <c r="P7" s="49"/>
       <c r="Q7" s="50"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="30" t="s">
         <v>108</v>
       </c>
@@ -2808,7 +2808,7 @@
       <c r="P8" s="49"/>
       <c r="Q8" s="50"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="37" t="s">
         <v>161</v>
       </c>
@@ -2831,7 +2831,7 @@
       <c r="P9" s="52"/>
       <c r="Q9" s="53"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="42" t="s">
         <v>82</v>
       </c>
@@ -2868,7 +2868,7 @@
       </c>
       <c r="Q10" s="34"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="30" t="s">
         <v>107</v>
       </c>
@@ -2905,7 +2905,7 @@
       </c>
       <c r="Q11" s="36"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="30" t="s">
         <v>108</v>
       </c>
@@ -2942,7 +2942,7 @@
       </c>
       <c r="Q12" s="36"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="37" t="s">
         <v>161</v>
       </c>
@@ -2965,7 +2965,7 @@
       <c r="P13" s="40"/>
       <c r="Q13" s="41"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="42" t="s">
         <v>82</v>
       </c>
@@ -2992,7 +2992,7 @@
       <c r="P14" s="33"/>
       <c r="Q14" s="34"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="30" t="s">
         <v>107</v>
       </c>
@@ -3018,7 +3018,7 @@
       <c r="P15" s="35"/>
       <c r="Q15" s="36"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="30" t="s">
         <v>108</v>
       </c>
@@ -3044,7 +3044,7 @@
       <c r="P16" s="35"/>
       <c r="Q16" s="36"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="37" t="s">
         <v>161</v>
       </c>
@@ -3069,7 +3069,7 @@
       <c r="P17" s="40"/>
       <c r="Q17" s="41"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="30" t="s">
         <v>82</v>
       </c>
@@ -3095,7 +3095,7 @@
       <c r="P18" s="35"/>
       <c r="Q18" s="36"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="30" t="s">
         <v>107</v>
       </c>
@@ -3121,7 +3121,7 @@
       <c r="P19" s="35"/>
       <c r="Q19" s="36"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="30" t="s">
         <v>108</v>
       </c>
@@ -3147,7 +3147,7 @@
       <c r="P20" s="35"/>
       <c r="Q20" s="36"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="37" t="s">
         <v>161</v>
       </c>
@@ -3186,17 +3186,17 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="56" t="s">
         <v>175</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -3234,7 +3234,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3248,7 +3248,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -3265,7 +3265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -3406,7 +3406,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -3420,7 +3420,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -3451,7 +3451,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>69</v>
       </c>

</xml_diff>

<commit_message>
added structure for spring and fall schedule. no more manual date generation
</commit_message>
<xml_diff>
--- a/data/AD698-Schedule.xlsx
+++ b/data/AD698-Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npadalka\Documents\Repositories\AD698-generative-ai-for-BA\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\AD698-generative-ai-for-BA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CB9708-DF79-429C-A3F0-7990A0884EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E613370-30EF-4F99-A650-208E8F24A883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" activeTab="2" xr2:uid="{289CF049-F2D7-49EE-A36E-C623D66A4696}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{289CF049-F2D7-49EE-A36E-C623D66A4696}"/>
   </bookViews>
   <sheets>
     <sheet name="Course Details" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="226">
   <si>
     <t>Assignment</t>
   </si>
@@ -717,6 +717,9 @@
   </si>
   <si>
     <t>Weekly Labs*</t>
+  </si>
+  <si>
+    <t>6:00PM</t>
   </si>
 </sst>
 </file>
@@ -1478,18 +1481,18 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="58" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" style="58" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="58" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" style="58" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.81640625" style="59" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1796875" style="58" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7265625" style="58" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="58"/>
+    <col min="4" max="4" width="52.85546875" style="59" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="58" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="58" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>175</v>
       </c>
@@ -1509,7 +1512,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1525,7 +1528,7 @@
       <c r="E2" s="60"/>
       <c r="F2" s="60"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1541,7 +1544,7 @@
       <c r="E3" s="60"/>
       <c r="F3" s="60"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1557,7 +1560,7 @@
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1573,7 +1576,7 @@
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1589,7 +1592,7 @@
       <c r="E6" s="60"/>
       <c r="F6" s="60"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1605,7 +1608,7 @@
       <c r="E7" s="60"/>
       <c r="F7" s="60"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1621,7 +1624,7 @@
       <c r="E8" s="60"/>
       <c r="F8" s="60"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1637,7 +1640,7 @@
       <c r="E9" s="60"/>
       <c r="F9" s="60"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1653,7 +1656,7 @@
       <c r="E10" s="60"/>
       <c r="F10" s="60"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1669,7 +1672,7 @@
       <c r="E11" s="60"/>
       <c r="F11" s="60"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -1685,7 +1688,7 @@
       <c r="E12" s="60"/>
       <c r="F12" s="60"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1701,7 +1704,7 @@
       <c r="E13" s="60"/>
       <c r="F13" s="60"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -1717,7 +1720,7 @@
       <c r="E14" s="60"/>
       <c r="F14" s="60"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1732,7 +1735,7 @@
       </c>
       <c r="E15" s="60"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -1747,7 +1750,7 @@
       </c>
       <c r="E16" s="60"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -1762,7 +1765,7 @@
       </c>
       <c r="E17" s="60"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -1777,7 +1780,7 @@
       </c>
       <c r="E18" s="60"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>69</v>
       </c>
@@ -1792,16 +1795,16 @@
       </c>
       <c r="E19" s="60"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E20" s="60"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E21" s="60"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E22" s="60"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E23" s="60"/>
     </row>
   </sheetData>
@@ -1813,21 +1816,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF015F21-B674-4B2F-B456-A6FAF27E0BC1}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="5"/>
+    <col min="2" max="2" width="27.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>77</v>
       </c>
@@ -1844,7 +1847,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
         <v>82</v>
       </c>
@@ -1857,11 +1860,11 @@
       <c r="D2" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="55">
-        <v>0.60416666666666663</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E2" s="55" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
         <v>85</v>
       </c>
@@ -1888,23 +1891,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC9F4A2C-504E-4299-BCAC-273B4ED698AA}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.26953125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="25.26953125" customWidth="1"/>
-    <col min="5" max="5" width="46.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.1796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.1796875" style="7" customWidth="1"/>
-    <col min="8" max="8" width="9.1796875" style="12"/>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="46.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -1927,7 +1930,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>95</v>
       </c>
@@ -1953,7 +1956,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>224</v>
       </c>
@@ -1979,7 +1982,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>97</v>
       </c>
@@ -2005,7 +2008,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -2031,7 +2034,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>106</v>
       </c>
@@ -2053,7 +2056,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E7" s="11" t="s">
         <v>100</v>
       </c>
@@ -2063,7 +2066,7 @@
       <c r="G7" s="9"/>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E8" s="11" t="s">
         <v>101</v>
       </c>
@@ -2073,7 +2076,7 @@
       <c r="G8" s="9"/>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E9" s="11" t="s">
         <v>102</v>
       </c>
@@ -2083,7 +2086,7 @@
       <c r="G9" s="9"/>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E10" s="11" t="s">
         <v>103</v>
       </c>
@@ -2093,7 +2096,7 @@
       <c r="G10" s="9"/>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>104</v>
       </c>
@@ -2108,7 +2111,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>105</v>
       </c>
@@ -2123,7 +2126,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E13" s="8" t="s">
         <v>106</v>
       </c>
@@ -2148,13 +2151,13 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>82</v>
       </c>
@@ -2165,7 +2168,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>45678</v>
       </c>
@@ -2176,7 +2179,7 @@
         <v>45679</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <f>A2+1</f>
         <v>45679</v>
@@ -2190,7 +2193,7 @@
         <v>45680</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <f t="shared" ref="A4:A8" si="1">A3+1</f>
         <v>45680</v>
@@ -2204,7 +2207,7 @@
         <v>45681</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <f t="shared" si="1"/>
         <v>45681</v>
@@ -2218,7 +2221,7 @@
         <v>45682</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <f t="shared" si="1"/>
         <v>45682</v>
@@ -2232,7 +2235,7 @@
         <v>45683</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <f t="shared" si="1"/>
         <v>45683</v>
@@ -2246,7 +2249,7 @@
         <v>45684</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <f t="shared" si="1"/>
         <v>45684</v>
@@ -2274,25 +2277,25 @@
       <selection activeCell="G3" sqref="G2:L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="11.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="11.7265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="10.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.26953125" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.1796875" style="20"/>
+    <col min="1" max="1" width="11.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="11.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="11.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="10.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>109</v>
       </c>
@@ -2354,7 +2357,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>128</v>
       </c>
@@ -2425,7 +2428,7 @@
         <v>46006</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>133</v>
       </c>
@@ -2476,13 +2479,13 @@
       <c r="S3" s="24"/>
       <c r="T3" s="24"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
       <c r="D4" s="21"/>
       <c r="E4" s="22"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B5" s="22"/>
       <c r="C5" s="22"/>
       <c r="D5" s="21"/>
@@ -2506,28 +2509,28 @@
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7265625" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.26953125" style="45" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.1796875" style="45" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" style="45" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" style="45" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="45" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.26953125" style="45" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.1796875" style="45" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.26953125" style="45" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" style="45" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="45" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" style="45" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" style="45" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.1796875" style="45" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.26953125" style="45" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.453125" style="45" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="45" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.28515625" style="45" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="45" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10" style="45" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.54296875" style="45" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.26953125" style="45" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.1796875" style="31"/>
+    <col min="15" max="16" width="10.5703125" style="45" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.28515625" style="45" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>135</v>
       </c>
@@ -2580,7 +2583,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>82</v>
       </c>
@@ -2621,7 +2624,7 @@
       <c r="P2" s="33"/>
       <c r="Q2" s="34"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>107</v>
       </c>
@@ -2662,7 +2665,7 @@
       <c r="P3" s="35"/>
       <c r="Q3" s="36"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>108</v>
       </c>
@@ -2703,7 +2706,7 @@
       <c r="P4" s="35"/>
       <c r="Q4" s="36"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
         <v>161</v>
       </c>
@@ -2726,7 +2729,7 @@
       <c r="P5" s="40"/>
       <c r="Q5" s="41"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="42" t="s">
         <v>82</v>
       </c>
@@ -2754,7 +2757,7 @@
       <c r="P6" s="47"/>
       <c r="Q6" s="48"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>107</v>
       </c>
@@ -2781,7 +2784,7 @@
       <c r="P7" s="49"/>
       <c r="Q7" s="50"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>108</v>
       </c>
@@ -2808,7 +2811,7 @@
       <c r="P8" s="49"/>
       <c r="Q8" s="50"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
         <v>161</v>
       </c>
@@ -2831,7 +2834,7 @@
       <c r="P9" s="52"/>
       <c r="Q9" s="53"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="42" t="s">
         <v>82</v>
       </c>
@@ -2868,7 +2871,7 @@
       </c>
       <c r="Q10" s="34"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>107</v>
       </c>
@@ -2905,7 +2908,7 @@
       </c>
       <c r="Q11" s="36"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>108</v>
       </c>
@@ -2942,7 +2945,7 @@
       </c>
       <c r="Q12" s="36"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="37" t="s">
         <v>161</v>
       </c>
@@ -2965,7 +2968,7 @@
       <c r="P13" s="40"/>
       <c r="Q13" s="41"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="42" t="s">
         <v>82</v>
       </c>
@@ -2992,7 +2995,7 @@
       <c r="P14" s="33"/>
       <c r="Q14" s="34"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>107</v>
       </c>
@@ -3018,7 +3021,7 @@
       <c r="P15" s="35"/>
       <c r="Q15" s="36"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>108</v>
       </c>
@@ -3044,7 +3047,7 @@
       <c r="P16" s="35"/>
       <c r="Q16" s="36"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
         <v>161</v>
       </c>
@@ -3069,7 +3072,7 @@
       <c r="P17" s="40"/>
       <c r="Q17" s="41"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
         <v>82</v>
       </c>
@@ -3095,7 +3098,7 @@
       <c r="P18" s="35"/>
       <c r="Q18" s="36"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>107</v>
       </c>
@@ -3121,7 +3124,7 @@
       <c r="P19" s="35"/>
       <c r="Q19" s="36"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
         <v>108</v>
       </c>
@@ -3147,7 +3150,7 @@
       <c r="P20" s="35"/>
       <c r="Q20" s="36"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="37" t="s">
         <v>161</v>
       </c>
@@ -3186,17 +3189,17 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>175</v>
       </c>
@@ -3216,7 +3219,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -3234,7 +3237,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3248,7 +3251,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -3265,7 +3268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -3279,7 +3282,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -3293,7 +3296,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -3313,7 +3316,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -3327,7 +3330,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -3344,7 +3347,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -3358,7 +3361,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -3375,7 +3378,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -3389,7 +3392,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -3406,7 +3409,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -3420,7 +3423,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -3437,7 +3440,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -3451,7 +3454,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -3471,7 +3474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -3485,7 +3488,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>69</v>
       </c>

</xml_diff>

<commit_message>
added bag of words in lecture 2
</commit_message>
<xml_diff>
--- a/data/AD698-Schedule.xlsx
+++ b/data/AD698-Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\AD698-generative-ai-for-BA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916DF95C-0A2B-4D63-BD1C-B5290CF99825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{54DE32E2-DB1D-4665-B724-925D94C4E6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{289CF049-F2D7-49EE-A36E-C623D66A4696}"/>
   </bookViews>
@@ -24,6 +24,7 @@
     <sheet name="Course Details (2)" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1696,7 +1697,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2444,85 +2445,85 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
-        <f>A2+1</f>
+        <f t="shared" ref="A3:A8" si="0">A2+1</f>
         <v>45679</v>
       </c>
       <c r="B3" s="14">
-        <f t="shared" ref="B3:C8" si="0">B2+1</f>
+        <f t="shared" ref="B3:C8" si="1">B2+1</f>
         <v>45681</v>
       </c>
       <c r="C3" s="14">
+        <f t="shared" si="1"/>
+        <v>45680</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
         <f t="shared" si="0"/>
         <v>45680</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
-        <f t="shared" ref="A4:A8" si="1">A3+1</f>
-        <v>45680</v>
-      </c>
       <c r="B4" s="14">
+        <f t="shared" si="1"/>
+        <v>45682</v>
+      </c>
+      <c r="C4" s="14">
+        <f t="shared" si="1"/>
+        <v>45681</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <f t="shared" si="0"/>
+        <v>45681</v>
+      </c>
+      <c r="B5" s="14">
+        <f t="shared" si="1"/>
+        <v>45683</v>
+      </c>
+      <c r="C5" s="14">
+        <f t="shared" si="1"/>
+        <v>45682</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
         <f t="shared" si="0"/>
         <v>45682</v>
       </c>
-      <c r="C4" s="14">
-        <f t="shared" si="0"/>
-        <v>45681</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="14">
+      <c r="B6" s="14">
         <f t="shared" si="1"/>
-        <v>45681</v>
-      </c>
-      <c r="B5" s="14">
+        <v>45684</v>
+      </c>
+      <c r="C6" s="14">
+        <f t="shared" si="1"/>
+        <v>45683</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
         <f t="shared" si="0"/>
         <v>45683</v>
       </c>
-      <c r="C5" s="14">
-        <f t="shared" si="0"/>
-        <v>45682</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
+      <c r="B7" s="14">
         <f t="shared" si="1"/>
-        <v>45682</v>
-      </c>
-      <c r="B6" s="14">
+        <v>45685</v>
+      </c>
+      <c r="C7" s="14">
+        <f t="shared" si="1"/>
+        <v>45684</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
         <f t="shared" si="0"/>
         <v>45684</v>
       </c>
-      <c r="C6" s="14">
-        <f t="shared" si="0"/>
-        <v>45683</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
+      <c r="B8" s="14">
         <f t="shared" si="1"/>
-        <v>45683</v>
-      </c>
-      <c r="B7" s="14">
-        <f t="shared" si="0"/>
-        <v>45685</v>
-      </c>
-      <c r="C7" s="14">
-        <f t="shared" si="0"/>
-        <v>45684</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
+        <v>45686</v>
+      </c>
+      <c r="C8" s="14">
         <f t="shared" si="1"/>
-        <v>45684</v>
-      </c>
-      <c r="B8" s="14">
-        <f t="shared" si="0"/>
-        <v>45686</v>
-      </c>
-      <c r="C8" s="14">
-        <f t="shared" si="0"/>
         <v>45685</v>
       </c>
     </row>
@@ -2643,11 +2644,11 @@
         <v>45908</v>
       </c>
       <c r="H2" s="24">
-        <f>G2+7</f>
+        <f t="shared" ref="H2:J3" si="0">G2+7</f>
         <v>45915</v>
       </c>
       <c r="I2" s="24">
-        <f t="shared" ref="I2:J3" si="0">H2+7</f>
+        <f t="shared" si="0"/>
         <v>45922</v>
       </c>
       <c r="J2" s="24">
@@ -2714,7 +2715,7 @@
         <v>45902</v>
       </c>
       <c r="H3" s="24">
-        <f>G3+7</f>
+        <f t="shared" si="0"/>
         <v>45909</v>
       </c>
       <c r="I3" s="24">
@@ -3449,7 +3450,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fixed pytorch cuda environment
</commit_message>
<xml_diff>
--- a/data/AD698-Schedule.xlsx
+++ b/data/AD698-Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\AD698-generative-ai-for-BA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{54DE32E2-DB1D-4665-B724-925D94C4E6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06401DB-C493-4D70-AC60-C315CCEFDBBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{289CF049-F2D7-49EE-A36E-C623D66A4696}"/>
+    <workbookView xWindow="-28920" yWindow="-225" windowWidth="29040" windowHeight="15720" xr2:uid="{289CF049-F2D7-49EE-A36E-C623D66A4696}"/>
   </bookViews>
   <sheets>
     <sheet name="Course Details" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,6 @@
     <sheet name="Course Details (2)" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -761,12 +760,6 @@
     <t>Group Paper Presentation (Once per Group)*</t>
   </si>
   <si>
-    <t>GitHub Education and Student Account Creations</t>
-  </si>
-  <si>
-    <t>GitHub, Github Classrooms; Jupyter Notebooks, Quarto overview; submitting practice files.</t>
-  </si>
-  <si>
     <t>Github Classrooms, Jupyter Notebooks, Quarto, and Portfolio</t>
   </si>
   <si>
@@ -936,6 +929,12 @@
   </si>
   <si>
     <t>Bender et al. (2021) Stochastic Parrots; Survey on Hallucination in LLMs; Responsible AI for Enterprise Systems</t>
+  </si>
+  <si>
+    <t>Google Cloud, GitHub, Other Student Account Creations</t>
+  </si>
+  <si>
+    <t>GitHub, Github Classrooms; Jupyter Notebooks, Quarto overview, Google Colab and cloud; submitting practice files.</t>
   </si>
 </sst>
 </file>
@@ -1697,7 +1696,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1717,7 +1716,7 @@
         <v>169</v>
       </c>
       <c r="B1" s="61" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C1" s="56" t="s">
         <v>5</v>
@@ -1735,21 +1734,21 @@
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>227</v>
       </c>
       <c r="B2" s="61" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C2" t="s">
         <v>174</v>
       </c>
       <c r="D2" s="57" t="s">
-        <v>238</v>
+        <v>295</v>
       </c>
       <c r="E2" s="57" t="s">
-        <v>239</v>
+        <v>296</v>
       </c>
       <c r="F2" s="60"/>
       <c r="G2" s="60"/>
@@ -1759,16 +1758,16 @@
         <v>227</v>
       </c>
       <c r="B3" s="61" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C3" t="s">
         <v>175</v>
       </c>
       <c r="D3" s="57" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E3" s="57" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F3" s="60"/>
       <c r="G3" s="60"/>
@@ -1778,16 +1777,16 @@
         <v>228</v>
       </c>
       <c r="B4" s="61" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C4" t="s">
         <v>176</v>
       </c>
       <c r="D4" s="61" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E4" s="61" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F4" s="60"/>
       <c r="G4" s="60"/>
@@ -1797,16 +1796,16 @@
         <v>228</v>
       </c>
       <c r="B5" s="61" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C5" t="s">
         <v>177</v>
       </c>
       <c r="D5" s="61" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E5" s="61" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F5" s="60"/>
       <c r="G5" s="60"/>
@@ -1816,7 +1815,7 @@
         <v>229</v>
       </c>
       <c r="B6" s="61" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C6" t="s">
         <v>178</v>
@@ -1825,7 +1824,7 @@
         <v>201</v>
       </c>
       <c r="E6" s="61" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F6" s="60"/>
       <c r="G6" s="60"/>
@@ -1835,7 +1834,7 @@
         <v>229</v>
       </c>
       <c r="B7" s="61" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C7" t="s">
         <v>179</v>
@@ -1844,7 +1843,7 @@
         <v>203</v>
       </c>
       <c r="E7" s="61" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F7" s="60"/>
       <c r="G7" s="60"/>
@@ -1854,7 +1853,7 @@
         <v>230</v>
       </c>
       <c r="B8" s="61" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C8" t="s">
         <v>180</v>
@@ -1863,7 +1862,7 @@
         <v>204</v>
       </c>
       <c r="E8" s="61" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F8" s="60"/>
       <c r="G8" s="60"/>
@@ -1873,16 +1872,16 @@
         <v>230</v>
       </c>
       <c r="B9" s="61" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C9" t="s">
         <v>181</v>
       </c>
       <c r="D9" s="61" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E9" s="61" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F9" s="60"/>
       <c r="G9" s="60"/>
@@ -1892,16 +1891,16 @@
         <v>231</v>
       </c>
       <c r="B10" s="61" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C10" t="s">
         <v>182</v>
       </c>
       <c r="D10" s="61" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E10" s="61" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F10" s="60"/>
       <c r="G10" s="60"/>
@@ -1911,7 +1910,7 @@
         <v>231</v>
       </c>
       <c r="B11" s="61" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C11" t="s">
         <v>183</v>
@@ -1920,7 +1919,7 @@
         <v>208</v>
       </c>
       <c r="E11" s="61" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F11" s="60"/>
       <c r="G11" s="60"/>
@@ -1930,16 +1929,16 @@
         <v>232</v>
       </c>
       <c r="B12" s="61" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C12" t="s">
         <v>184</v>
       </c>
       <c r="D12" s="61" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E12" s="61" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F12" s="60"/>
       <c r="G12" s="60"/>
@@ -1949,16 +1948,16 @@
         <v>232</v>
       </c>
       <c r="B13" s="61" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C13" t="s">
         <v>185</v>
       </c>
       <c r="D13" s="61" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E13" s="61" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F13" s="60"/>
       <c r="G13" s="60"/>
@@ -1968,16 +1967,16 @@
         <v>233</v>
       </c>
       <c r="B14" s="61" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C14" t="s">
         <v>186</v>
       </c>
       <c r="D14" s="61" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E14" s="61" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F14" s="60"/>
       <c r="G14" s="60"/>
@@ -1987,16 +1986,16 @@
         <v>233</v>
       </c>
       <c r="B15" s="61" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C15" t="s">
         <v>187</v>
       </c>
       <c r="D15" s="61" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E15" s="61" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F15" s="60"/>
     </row>
@@ -2005,16 +2004,16 @@
         <v>234</v>
       </c>
       <c r="B16" s="61" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C16" t="s">
         <v>188</v>
       </c>
       <c r="D16" s="61" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E16" s="61" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F16" s="60"/>
     </row>
@@ -2023,7 +2022,7 @@
         <v>234</v>
       </c>
       <c r="B17" s="61" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C17" t="s">
         <v>189</v>
@@ -2032,7 +2031,7 @@
         <v>216</v>
       </c>
       <c r="E17" s="61" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F17" s="60"/>
     </row>
@@ -2041,7 +2040,7 @@
         <v>235</v>
       </c>
       <c r="B18" s="61" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C18" t="s">
         <v>190</v>
@@ -2050,7 +2049,7 @@
         <v>218</v>
       </c>
       <c r="E18" s="61" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F18" s="60"/>
     </row>
@@ -2059,16 +2058,16 @@
         <v>235</v>
       </c>
       <c r="B19" s="61" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C19" t="s">
         <v>191</v>
       </c>
       <c r="D19" s="61" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E19" s="61" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F19" s="60"/>
     </row>
@@ -3785,97 +3784,97 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated module 0 topics to contain colab
</commit_message>
<xml_diff>
--- a/data/AD698-Schedule.xlsx
+++ b/data/AD698-Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\AD698-generative-ai-for-BA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06401DB-C493-4D70-AC60-C315CCEFDBBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DEE542-5B75-4491-A057-2B6E3ADB697E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-225" windowWidth="29040" windowHeight="15720" xr2:uid="{289CF049-F2D7-49EE-A36E-C623D66A4696}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{289CF049-F2D7-49EE-A36E-C623D66A4696}"/>
   </bookViews>
   <sheets>
     <sheet name="Course Details" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="277">
   <si>
     <t>Assignment</t>
   </si>
@@ -640,93 +640,24 @@
     <t>Grounded Generation &amp; Guardrails</t>
   </si>
   <si>
-    <t>Course Orientation &amp; Reproducible GenAI Setup</t>
-  </si>
-  <si>
-    <t>Course overview; GitHub Classroom; Quarto/Jupyter workflows; version control; AI disclosure files; reproducibility expectations.</t>
-  </si>
-  <si>
-    <t>Why language is probabilistic; prediction as generation; uncertainty in text; why NLP is the foundation of modern GenAI.</t>
-  </si>
-  <si>
     <t>Mathematical Foundations Through Language Modeling</t>
   </si>
   <si>
-    <t>Vectors as meaning; probability and conditional likelihood in language models; loss functions; entropy and perplexity introduced through NLP.</t>
-  </si>
-  <si>
     <t>From Words to Structured Text</t>
   </si>
   <si>
     <t>Prompting as System Design</t>
   </si>
   <si>
-    <t>Prompt engineering as probabilistic control; zero/few-shot prompting; in-context learning; prompt failure modes in regulated text.</t>
-  </si>
-  <si>
-    <t>Subword tokenization; embedding spaces; cosine similarity; semantic neighborhoods; disclosure similarity and drift.</t>
-  </si>
-  <si>
-    <t>Self-attention; positional encoding; scaling laws; why transformers replaced RNNs and LSTMs.</t>
-  </si>
-  <si>
     <t>Training Paradigms and Fine-Tuning Pipelines</t>
   </si>
   <si>
-    <t>Pretraining vs fine-tuning; instruction tuning; dataset formatting; risks of overfitting and data leakage.</t>
-  </si>
-  <si>
-    <t>Retrieval-Augmented Generation Concepts</t>
-  </si>
-  <si>
-    <t>Chunking strategies; indexing; embedding-based retrieval; grounding and hallucination risks in enterprise GenAI.</t>
-  </si>
-  <si>
-    <t>Designing RAG Pipelines for SEC Disclosures</t>
-  </si>
-  <si>
-    <t>End-to-end RAG workflows over 10-Ks; query design; citation tracing; limitations of retrieval-based systems.</t>
-  </si>
-  <si>
-    <t>Embedding-based clustering; similarity search; longitudinal semantic change analysis across filings.</t>
-  </si>
-  <si>
-    <t>Context limitations; summarization; caching; memory strategies for long regulatory documents.</t>
-  </si>
-  <si>
     <t>Multimodal Generative Models and Structured Data</t>
   </si>
   <si>
-    <t>Vision-language models; tables and figures in filings; multimodal futures for enterprise GenAI.</t>
-  </si>
-  <si>
     <t>Evaluating Generative AI Systems</t>
   </si>
   <si>
-    <t>Language, Probability, and Generative Systems</t>
-  </si>
-  <si>
-    <t>NLP foundations: tokenization, normalization, n-grams, static vs contextual representations; SEC 10-K document structure.</t>
-  </si>
-  <si>
-    <t>Tokenization, Embeddings, and Semantic Geometry</t>
-  </si>
-  <si>
-    <t>Transformers, Attention, and Context</t>
-  </si>
-  <si>
-    <t>Efficient Adaptation: LoRA, QLoRA, and PEFT</t>
-  </si>
-  <si>
-    <t>Parameter-efficient fine-tuning; tradeoffs between prompting, RAG, and adaptation; cost and governance considerations.</t>
-  </si>
-  <si>
-    <t>Semantic Search, Clustering, and Change Detection</t>
-  </si>
-  <si>
-    <t>Context Windows, Memory, and Compression</t>
-  </si>
-  <si>
     <t>M0</t>
   </si>
   <si>
@@ -760,12 +691,6 @@
     <t>Group Paper Presentation (Once per Group)*</t>
   </si>
   <si>
-    <t>Github Classrooms, Jupyter Notebooks, Quarto, and Portfolio</t>
-  </si>
-  <si>
-    <t>Development environment setup; Explanation of portfolio submissions and group assignments.</t>
-  </si>
-  <si>
     <t>Week</t>
   </si>
   <si>
@@ -931,10 +856,25 @@
     <t>Bender et al. (2021) Stochastic Parrots; Survey on Hallucination in LLMs; Responsible AI for Enterprise Systems</t>
   </si>
   <si>
-    <t>Google Cloud, GitHub, Other Student Account Creations</t>
-  </si>
-  <si>
-    <t>GitHub, Github Classrooms; Jupyter Notebooks, Quarto overview, Google Colab and cloud; submitting practice files.</t>
+    <t>Google Colab &amp; Execution Environment Setup with technical orientation</t>
+  </si>
+  <si>
+    <t>Google Colab setup; notebook fundamentals; Python runtime basics; managing files, sessions, and outputs; running, saving, exporting, and submitting notebooks.</t>
+  </si>
+  <si>
+    <t>Optional GitHub Classroom &amp; Version Control Basics 	Optional GitHub account setup</t>
+  </si>
+  <si>
+    <t>GitHub Classroom workflow; cloning and opening notebooks in Colab; basic version control concepts (commit, push, pull); when and why GitHub is used in applied GenAI work.</t>
+  </si>
+  <si>
+    <t>L0.3</t>
+  </si>
+  <si>
+    <t>Overview of GenAI technical stack, GenAI Tooling, APIs, and Responsible Usage Foundations.</t>
+  </si>
+  <si>
+    <t>LLM APIs (OpenAI, Gemini, Anthropic); prompt execution vs programmatic calls; API keys and secrets management; cost awareness; responsible and accountable GenAI usage.</t>
   </si>
 </sst>
 </file>
@@ -946,7 +886,7 @@
     <numFmt numFmtId="165" formatCode="ddd"/>
     <numFmt numFmtId="166" formatCode="d\-mmm\ \(ddd\)"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1036,6 +976,12 @@
     <font>
       <sz val="9"/>
       <color rgb="FF00B050"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1179,7 +1125,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1346,17 +1292,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1693,30 +1636,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B2A5D89-D79C-44C1-8747-841FF0601386}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="58" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="8" style="58" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="88" style="59" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="58"/>
+    <col min="1" max="1" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" style="4" customWidth="1"/>
+    <col min="3" max="3" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="88" style="60" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="61" t="s">
-        <v>267</v>
+      <c r="B1" s="60" t="s">
+        <v>242</v>
       </c>
       <c r="C1" s="56" t="s">
         <v>5</v>
@@ -1735,360 +1678,355 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="60" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>272</v>
+      </c>
+      <c r="E2" s="57" t="s">
+        <v>273</v>
+      </c>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" s="60" t="s">
+        <v>243</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="57" t="s">
+        <v>270</v>
+      </c>
+      <c r="E3" s="57" t="s">
+        <v>271</v>
+      </c>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B4" s="60" t="s">
+        <v>244</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D4" s="60" t="s">
+        <v>216</v>
+      </c>
+      <c r="E4" s="60" t="s">
+        <v>241</v>
+      </c>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B5" s="60" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D5" s="60" t="s">
+        <v>217</v>
+      </c>
+      <c r="E5" s="60" t="s">
+        <v>218</v>
+      </c>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" s="60" t="s">
+        <v>245</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>198</v>
+      </c>
+      <c r="E6" s="60" t="s">
+        <v>219</v>
+      </c>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B7" s="60" t="s">
+        <v>245</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D7" s="60" t="s">
+        <v>199</v>
+      </c>
+      <c r="E7" s="60" t="s">
+        <v>220</v>
+      </c>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B8" s="60" t="s">
+        <v>246</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D8" s="60" t="s">
+        <v>200</v>
+      </c>
+      <c r="E8" s="60" t="s">
+        <v>221</v>
+      </c>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B9" s="60" t="s">
+        <v>246</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D9" s="60" t="s">
+        <v>222</v>
+      </c>
+      <c r="E9" s="60" t="s">
+        <v>223</v>
+      </c>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B10" s="60" t="s">
+        <v>247</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D10" s="60" t="s">
+        <v>224</v>
+      </c>
+      <c r="E10" s="60" t="s">
+        <v>225</v>
+      </c>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B11" s="60" t="s">
+        <v>247</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D11" s="60" t="s">
+        <v>201</v>
+      </c>
+      <c r="E11" s="60" t="s">
+        <v>226</v>
+      </c>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B12" s="60" t="s">
+        <v>248</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D12" s="60" t="s">
         <v>227</v>
       </c>
-      <c r="B2" s="61" t="s">
-        <v>268</v>
-      </c>
-      <c r="C2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D2" s="57" t="s">
-        <v>295</v>
-      </c>
-      <c r="E2" s="57" t="s">
-        <v>296</v>
-      </c>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>227</v>
-      </c>
-      <c r="B3" s="61" t="s">
-        <v>268</v>
-      </c>
-      <c r="C3" t="s">
-        <v>175</v>
-      </c>
-      <c r="D3" s="57" t="s">
+      <c r="E12" s="60" t="s">
+        <v>228</v>
+      </c>
+      <c r="F12" s="58"/>
+      <c r="G12" s="58"/>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B13" s="60" t="s">
+        <v>248</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D13" s="60" t="s">
+        <v>229</v>
+      </c>
+      <c r="E13" s="60" t="s">
+        <v>230</v>
+      </c>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B14" s="60" t="s">
+        <v>249</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D14" s="60" t="s">
+        <v>231</v>
+      </c>
+      <c r="E14" s="60" t="s">
+        <v>232</v>
+      </c>
+      <c r="F14" s="58"/>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B15" s="60" t="s">
+        <v>249</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D15" s="60" t="s">
+        <v>233</v>
+      </c>
+      <c r="E15" s="60" t="s">
+        <v>234</v>
+      </c>
+      <c r="F15" s="58"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B16" s="60" t="s">
+        <v>250</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D16" s="60" t="s">
+        <v>235</v>
+      </c>
+      <c r="E16" s="60" t="s">
+        <v>236</v>
+      </c>
+      <c r="F16" s="58"/>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B17" s="60" t="s">
+        <v>250</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D17" s="60" t="s">
+        <v>202</v>
+      </c>
+      <c r="E17" s="60" t="s">
+        <v>237</v>
+      </c>
+      <c r="F17" s="58"/>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B18" s="60" t="s">
+        <v>251</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D18" s="60" t="s">
+        <v>203</v>
+      </c>
+      <c r="E18" s="60" t="s">
         <v>238</v>
       </c>
-      <c r="E3" s="57" t="s">
+      <c r="F18" s="58"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B19" s="60" t="s">
+        <v>251</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D19" s="60" t="s">
         <v>239</v>
       </c>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>228</v>
-      </c>
-      <c r="B4" s="61" t="s">
-        <v>269</v>
-      </c>
-      <c r="C4" t="s">
-        <v>176</v>
-      </c>
-      <c r="D4" s="61" t="s">
-        <v>241</v>
-      </c>
-      <c r="E4" s="61" t="s">
-        <v>266</v>
-      </c>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>228</v>
-      </c>
-      <c r="B5" s="61" t="s">
-        <v>269</v>
-      </c>
-      <c r="C5" t="s">
-        <v>177</v>
-      </c>
-      <c r="D5" s="61" t="s">
-        <v>242</v>
-      </c>
-      <c r="E5" s="61" t="s">
-        <v>243</v>
-      </c>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>229</v>
-      </c>
-      <c r="B6" s="61" t="s">
-        <v>270</v>
-      </c>
-      <c r="C6" t="s">
-        <v>178</v>
-      </c>
-      <c r="D6" s="61" t="s">
-        <v>201</v>
-      </c>
-      <c r="E6" s="61" t="s">
-        <v>244</v>
-      </c>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>229</v>
-      </c>
-      <c r="B7" s="61" t="s">
-        <v>270</v>
-      </c>
-      <c r="C7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D7" s="61" t="s">
-        <v>203</v>
-      </c>
-      <c r="E7" s="61" t="s">
-        <v>245</v>
-      </c>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>230</v>
-      </c>
-      <c r="B8" s="61" t="s">
-        <v>271</v>
-      </c>
-      <c r="C8" t="s">
-        <v>180</v>
-      </c>
-      <c r="D8" s="61" t="s">
-        <v>204</v>
-      </c>
-      <c r="E8" s="61" t="s">
-        <v>246</v>
-      </c>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>230</v>
-      </c>
-      <c r="B9" s="61" t="s">
-        <v>271</v>
-      </c>
-      <c r="C9" t="s">
-        <v>181</v>
-      </c>
-      <c r="D9" s="61" t="s">
-        <v>247</v>
-      </c>
-      <c r="E9" s="61" t="s">
-        <v>248</v>
-      </c>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>231</v>
-      </c>
-      <c r="B10" s="61" t="s">
-        <v>272</v>
-      </c>
-      <c r="C10" t="s">
-        <v>182</v>
-      </c>
-      <c r="D10" s="61" t="s">
-        <v>249</v>
-      </c>
-      <c r="E10" s="61" t="s">
-        <v>250</v>
-      </c>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>231</v>
-      </c>
-      <c r="B11" s="61" t="s">
-        <v>272</v>
-      </c>
-      <c r="C11" t="s">
-        <v>183</v>
-      </c>
-      <c r="D11" s="61" t="s">
-        <v>208</v>
-      </c>
-      <c r="E11" s="61" t="s">
-        <v>251</v>
-      </c>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>232</v>
-      </c>
-      <c r="B12" s="61" t="s">
-        <v>273</v>
-      </c>
-      <c r="C12" t="s">
-        <v>184</v>
-      </c>
-      <c r="D12" s="61" t="s">
-        <v>252</v>
-      </c>
-      <c r="E12" s="61" t="s">
-        <v>253</v>
-      </c>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>232</v>
-      </c>
-      <c r="B13" s="61" t="s">
-        <v>273</v>
-      </c>
-      <c r="C13" t="s">
-        <v>185</v>
-      </c>
-      <c r="D13" s="61" t="s">
-        <v>254</v>
-      </c>
-      <c r="E13" s="61" t="s">
-        <v>255</v>
-      </c>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-    </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>233</v>
-      </c>
-      <c r="B14" s="61" t="s">
-        <v>274</v>
-      </c>
-      <c r="C14" t="s">
-        <v>186</v>
-      </c>
-      <c r="D14" s="61" t="s">
-        <v>256</v>
-      </c>
-      <c r="E14" s="61" t="s">
-        <v>257</v>
-      </c>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>233</v>
-      </c>
-      <c r="B15" s="61" t="s">
-        <v>274</v>
-      </c>
-      <c r="C15" t="s">
-        <v>187</v>
-      </c>
-      <c r="D15" s="61" t="s">
-        <v>258</v>
-      </c>
-      <c r="E15" s="61" t="s">
-        <v>259</v>
-      </c>
-      <c r="F15" s="60"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>234</v>
-      </c>
-      <c r="B16" s="61" t="s">
-        <v>275</v>
-      </c>
-      <c r="C16" t="s">
-        <v>188</v>
-      </c>
-      <c r="D16" s="61" t="s">
-        <v>260</v>
-      </c>
-      <c r="E16" s="61" t="s">
-        <v>261</v>
-      </c>
-      <c r="F16" s="60"/>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>234</v>
-      </c>
-      <c r="B17" s="61" t="s">
-        <v>275</v>
-      </c>
-      <c r="C17" t="s">
-        <v>189</v>
-      </c>
-      <c r="D17" s="61" t="s">
-        <v>216</v>
-      </c>
-      <c r="E17" s="61" t="s">
-        <v>262</v>
-      </c>
-      <c r="F17" s="60"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>235</v>
-      </c>
-      <c r="B18" s="61" t="s">
-        <v>276</v>
-      </c>
-      <c r="C18" t="s">
-        <v>190</v>
-      </c>
-      <c r="D18" s="61" t="s">
-        <v>218</v>
-      </c>
-      <c r="E18" s="61" t="s">
-        <v>263</v>
-      </c>
-      <c r="F18" s="60"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>235</v>
-      </c>
-      <c r="B19" s="61" t="s">
-        <v>276</v>
-      </c>
-      <c r="C19" t="s">
-        <v>191</v>
-      </c>
-      <c r="D19" s="61" t="s">
-        <v>264</v>
-      </c>
-      <c r="E19" s="61" t="s">
-        <v>265</v>
-      </c>
-      <c r="F19" s="60"/>
+      <c r="E19" s="60" t="s">
+        <v>240</v>
+      </c>
+      <c r="F19" s="58"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20" s="60"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="58"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21" s="60"/>
+      <c r="F21" s="58"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F22" s="60"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F23" s="60"/>
+      <c r="F22" s="58"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2146,7 +2084,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
-        <v>236</v>
+        <v>213</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>167</v>
@@ -2247,7 +2185,7 @@
         <v>50</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>237</v>
+        <v>214</v>
       </c>
       <c r="F3" s="7">
         <v>1</v>
@@ -3784,97 +3722,97 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>278</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>279</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>282</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>283</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>284</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>285</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>287</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>288</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>289</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>290</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>291</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>292</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>293</v>
+        <v>268</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>294</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -3884,305 +3822,412 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64798F98-936B-4105-A1E0-B80F81BB3320}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="58" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="58" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="88" style="59" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="58"/>
+    <col min="1" max="1" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" style="5" customWidth="1"/>
+    <col min="3" max="3" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="88" style="60" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="59" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="D1" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="E1" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>272</v>
+      </c>
+      <c r="E2" s="57" t="s">
+        <v>273</v>
+      </c>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>243</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="57" t="s">
+        <v>270</v>
+      </c>
+      <c r="E3" s="57" t="s">
+        <v>271</v>
+      </c>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>243</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="E4" s="60" t="s">
+        <v>276</v>
+      </c>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" s="59" t="s">
+        <v>216</v>
+      </c>
+      <c r="E5" s="59" t="s">
+        <v>241</v>
+      </c>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>244</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D6" s="59" t="s">
+        <v>217</v>
+      </c>
+      <c r="E6" s="59" t="s">
+        <v>218</v>
+      </c>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>245</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D7" s="59" t="s">
+        <v>198</v>
+      </c>
+      <c r="E7" s="59" t="s">
+        <v>219</v>
+      </c>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B8" s="59" t="s">
+        <v>245</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D8" s="59" t="s">
+        <v>199</v>
+      </c>
+      <c r="E8" s="59" t="s">
+        <v>220</v>
+      </c>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>246</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D9" s="59" t="s">
+        <v>200</v>
+      </c>
+      <c r="E9" s="59" t="s">
+        <v>221</v>
+      </c>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B10" s="59" t="s">
+        <v>246</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="D10" s="59" t="s">
+        <v>222</v>
+      </c>
+      <c r="E10" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B11" s="59" t="s">
+        <v>247</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D11" s="59" t="s">
+        <v>224</v>
+      </c>
+      <c r="E11" s="59" t="s">
+        <v>225</v>
+      </c>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B12" s="59" t="s">
+        <v>247</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D12" s="59" t="s">
+        <v>201</v>
+      </c>
+      <c r="E12" s="59" t="s">
+        <v>226</v>
+      </c>
+      <c r="F12" s="58"/>
+      <c r="G12" s="58"/>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B13" s="59" t="s">
+        <v>248</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D13" s="59" t="s">
         <v>227</v>
       </c>
-      <c r="B2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>227</v>
-      </c>
-      <c r="B3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C3" t="s">
-        <v>219</v>
-      </c>
-      <c r="D3" t="s">
-        <v>200</v>
-      </c>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E13" s="59" t="s">
         <v>228</v>
       </c>
-      <c r="B4" t="s">
-        <v>176</v>
-      </c>
-      <c r="C4" t="s">
-        <v>201</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B14" s="59" t="s">
+        <v>248</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D14" s="59" t="s">
+        <v>229</v>
+      </c>
+      <c r="E14" s="59" t="s">
+        <v>230</v>
+      </c>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B15" s="59" t="s">
+        <v>249</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D15" s="59" t="s">
+        <v>231</v>
+      </c>
+      <c r="E15" s="59" t="s">
+        <v>232</v>
+      </c>
+      <c r="F15" s="58"/>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B16" s="59" t="s">
+        <v>249</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D16" s="59" t="s">
+        <v>233</v>
+      </c>
+      <c r="E16" s="59" t="s">
+        <v>234</v>
+      </c>
+      <c r="F16" s="58"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B17" s="59" t="s">
+        <v>250</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="E17" s="59" t="s">
+        <v>236</v>
+      </c>
+      <c r="F17" s="58"/>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B18" s="59" t="s">
+        <v>250</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D18" s="59" t="s">
         <v>202</v>
       </c>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>228</v>
-      </c>
-      <c r="B5" t="s">
-        <v>177</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E18" s="59" t="s">
+        <v>237</v>
+      </c>
+      <c r="F18" s="58"/>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B19" s="59" t="s">
+        <v>251</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D19" s="59" t="s">
         <v>203</v>
       </c>
-      <c r="D5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>229</v>
-      </c>
-      <c r="B6" t="s">
-        <v>178</v>
-      </c>
-      <c r="C6" t="s">
-        <v>204</v>
-      </c>
-      <c r="D6" t="s">
-        <v>205</v>
-      </c>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>229</v>
-      </c>
-      <c r="B7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C7" t="s">
-        <v>221</v>
-      </c>
-      <c r="D7" t="s">
-        <v>206</v>
-      </c>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>230</v>
-      </c>
-      <c r="B8" t="s">
-        <v>180</v>
-      </c>
-      <c r="C8" t="s">
-        <v>222</v>
-      </c>
-      <c r="D8" t="s">
-        <v>207</v>
-      </c>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>230</v>
-      </c>
-      <c r="B9" t="s">
-        <v>181</v>
-      </c>
-      <c r="C9" t="s">
-        <v>208</v>
-      </c>
-      <c r="D9" t="s">
-        <v>209</v>
-      </c>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>231</v>
-      </c>
-      <c r="B10" t="s">
-        <v>182</v>
-      </c>
-      <c r="C10" t="s">
-        <v>210</v>
-      </c>
-      <c r="D10" t="s">
-        <v>211</v>
-      </c>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>231</v>
-      </c>
-      <c r="B11" t="s">
-        <v>183</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="E19" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="F19" s="58"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="D11" t="s">
-        <v>213</v>
-      </c>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>232</v>
-      </c>
-      <c r="B12" t="s">
-        <v>184</v>
-      </c>
-      <c r="C12" t="s">
-        <v>223</v>
-      </c>
-      <c r="D12" t="s">
-        <v>224</v>
-      </c>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>232</v>
-      </c>
-      <c r="B13" t="s">
-        <v>185</v>
-      </c>
-      <c r="C13" t="s">
-        <v>225</v>
-      </c>
-      <c r="D13" t="s">
-        <v>214</v>
-      </c>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>233</v>
-      </c>
-      <c r="B14" t="s">
-        <v>186</v>
-      </c>
-      <c r="C14" t="s">
-        <v>226</v>
-      </c>
-      <c r="D14" t="s">
-        <v>215</v>
-      </c>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>233</v>
-      </c>
-      <c r="B15" t="s">
-        <v>187</v>
-      </c>
-      <c r="C15" t="s">
-        <v>216</v>
-      </c>
-      <c r="D15" t="s">
-        <v>217</v>
-      </c>
-      <c r="E15" s="60"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16" s="60"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17" s="60"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18" s="60"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19" s="60"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="60"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="60"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E22" s="60"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E23" s="60"/>
+      <c r="B20" s="59" t="s">
+        <v>251</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D20" s="59" t="s">
+        <v>239</v>
+      </c>
+      <c r="E20" s="59" t="s">
+        <v>240</v>
+      </c>
+      <c r="F20" s="58"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="58"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="58"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="58"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>